<commit_message>
Adding extract values from excel file to add book api example
</commit_message>
<xml_diff>
--- a/APIAutomation/src/excelDataDriven/ExcelBook.xlsx
+++ b/APIAutomation/src/excelDataDriven/ExcelBook.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Data1</t>
   </si>
@@ -79,6 +79,15 @@
   </si>
   <si>
     <t>TestCases</t>
+  </si>
+  <si>
+    <t>RestAddbook</t>
+  </si>
+  <si>
+    <t>RestAssured</t>
+  </si>
+  <si>
+    <t>asfasf</t>
   </si>
 </sst>
 </file>
@@ -407,8 +416,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -483,6 +492,20 @@
         <v>17</v>
       </c>
       <c r="F5" s="1"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6">
+        <v>3221</v>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="G14" s="1"/>

</xml_diff>